<commit_message>
Registro de nota completo
</commit_message>
<xml_diff>
--- a/Plantilla Seguimiento TP-Plan Entrega con comentarios 2016.xlsx
+++ b/Plantilla Seguimiento TP-Plan Entrega con comentarios 2016.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FFE1A7-F3A0-4DF3-B8D9-E60FB946150D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376F0364-C14E-489B-8A74-0A2ED6B19B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +236,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -346,6 +358,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,14 +388,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="D10:G17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="D24:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,15 +759,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -768,14 +798,14 @@
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="18">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="19" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="26" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="5"/>
@@ -784,163 +814,163 @@
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="20"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="20"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="20"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>3.8</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="18">
         <v>1</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="22"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="22" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="22"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="22" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23" t="s">
+      <c r="E12" s="15"/>
+      <c r="F12" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="22"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="2:8" s="2" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="22" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="24" t="s">
+      <c r="E13" s="15"/>
+      <c r="F13" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="2:8" s="2" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="22" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="24" t="s">
+      <c r="E14" s="15"/>
+      <c r="F14" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="22"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="19"/>
+      <c r="D15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="22"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="22" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="22"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="2:7" s="2" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="22" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23" t="s">
+      <c r="E17" s="15"/>
+      <c r="F17" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="22"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="2:7" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>3.14</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="18">
         <v>3</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -954,7 +984,7 @@
       <c r="B19" s="4">
         <v>3.15</v>
       </c>
-      <c r="C19" s="16"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="5" t="s">
         <v>16</v>
       </c>
@@ -966,7 +996,7 @@
       <c r="B20" s="4">
         <v>3.16</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="5" t="s">
         <v>17</v>
       </c>
@@ -980,7 +1010,7 @@
       <c r="B21" s="4">
         <v>3.18</v>
       </c>
-      <c r="C21" s="16"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="5" t="s">
         <v>18</v>
       </c>
@@ -990,19 +1020,19 @@
     </row>
     <row r="22" spans="2:7" s="2" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="12" t="s">
+      <c r="E22" s="15"/>
+      <c r="F22" s="16" t="s">
         <v>52</v>
       </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="2:7" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="16"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="2" t="s">
         <v>43</v>
       </c>
@@ -1014,74 +1044,74 @@
     </row>
     <row r="24" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="16"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="22" t="s">
         <v>51</v>
       </c>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="16"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="20"/>
+      <c r="F25" s="23"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="16"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="20"/>
+      <c r="F26" s="23"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="16"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="20"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="5" t="s">
+      <c r="C28" s="19"/>
+      <c r="D28" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="20"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
-      <c r="C29" s="16"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="20"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="20"/>
+      <c r="D30" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="21"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="2:7" ht="120" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Limpiar post eliminacion de alumno
</commit_message>
<xml_diff>
--- a/Plantilla Seguimiento TP-Plan Entrega con comentarios 2016.xlsx
+++ b/Plantilla Seguimiento TP-Plan Entrega con comentarios 2016.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224175F8-86DD-487D-894B-FEDA7AD2A1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C951FD50-AC50-497B-9BD1-263476013003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trabajo de Diploma" sheetId="2" r:id="rId1"/>
@@ -220,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,12 +236,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -362,9 +356,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -737,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,15 +741,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -789,14 +780,14 @@
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>2</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="15"/>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="5"/>
@@ -805,55 +796,55 @@
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="15"/>
-      <c r="F6" s="25"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="25"/>
+      <c r="F7" s="24"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="25"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="26"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>3.8</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="19">
         <v>1</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -867,7 +858,7 @@
       <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="15" t="s">
         <v>20</v>
       </c>
@@ -881,7 +872,7 @@
       <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="15" t="s">
         <v>31</v>
       </c>
@@ -895,7 +886,7 @@
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="15" t="s">
         <v>21</v>
       </c>
@@ -909,7 +900,7 @@
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="15" t="s">
         <v>38</v>
       </c>
@@ -923,7 +914,7 @@
       <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="15" t="s">
         <v>22</v>
       </c>
@@ -935,7 +926,7 @@
       <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="21"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="15" t="s">
         <v>23</v>
       </c>
@@ -947,7 +938,7 @@
       <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="15" t="s">
         <v>24</v>
       </c>
@@ -961,7 +952,7 @@
       <c r="B18" s="4">
         <v>3.14</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <v>3</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -975,7 +966,7 @@
       <c r="B19" s="4">
         <v>3.15</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="5" t="s">
         <v>16</v>
       </c>
@@ -987,12 +978,12 @@
       <c r="B20" s="4">
         <v>3.16</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="5" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="12" t="s">
+      <c r="E20" s="15"/>
+      <c r="F20" s="16" t="s">
         <v>56</v>
       </c>
       <c r="G20" s="5"/>
@@ -1001,7 +992,7 @@
       <c r="B21" s="4">
         <v>3.18</v>
       </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="5" t="s">
         <v>18</v>
       </c>
@@ -1011,7 +1002,7 @@
     </row>
     <row r="22" spans="2:7" s="2" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="21"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="18" t="s">
         <v>42</v>
       </c>
@@ -1023,7 +1014,7 @@
     </row>
     <row r="23" spans="2:7" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="21"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="18" t="s">
         <v>43</v>
       </c>
@@ -1035,74 +1026,74 @@
     </row>
     <row r="24" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="21"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="26" t="s">
         <v>51</v>
       </c>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="21"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="28"/>
+      <c r="F25" s="27"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="21"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="28"/>
+      <c r="F26" s="27"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="21"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="28"/>
+      <c r="F27" s="27"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="19" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="28"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="5" t="s">
+      <c r="C29" s="20"/>
+      <c r="D29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="28"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="27"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
-      <c r="C30" s="22"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E30" s="15"/>
-      <c r="F30" s="29"/>
+      <c r="F30" s="28"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="2:7" ht="120" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mejoras en el restore
</commit_message>
<xml_diff>
--- a/Plantilla Seguimiento TP-Plan Entrega con comentarios 2016.xlsx
+++ b/Plantilla Seguimiento TP-Plan Entrega con comentarios 2016.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6587C091-A619-4AE0-8B84-4E4B77CFB333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EE086D-7B6A-49C6-A2EA-935F52324A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -338,9 +338,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -377,15 +374,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -728,28 +716,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:F30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49" style="14" customWidth="1"/>
+    <col min="6" max="6" width="49" style="13" customWidth="1"/>
     <col min="7" max="7" width="56.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -780,14 +768,14 @@
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>2</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="23" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="22" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="5"/>
@@ -796,194 +784,194 @@
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="24"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="15" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="24"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="15" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="24"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>3.8</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="18">
         <v>1</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="15" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16" t="s">
+      <c r="E11" s="14"/>
+      <c r="F11" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="15" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16" t="s">
+      <c r="E12" s="14"/>
+      <c r="F12" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="2:8" s="2" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="15" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="17" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="2:8" s="2" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="17" t="s">
+      <c r="E14" s="14"/>
+      <c r="F14" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="15" t="s">
+      <c r="C15" s="19"/>
+      <c r="D15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="15"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="2:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="15" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="15"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="2:7" s="2" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="15" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16" t="s">
+      <c r="E17" s="14"/>
+      <c r="F17" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="15"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="2:7" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>3.14</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="18">
         <v>3</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="2:7" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>3.15</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="15" t="s">
+      <c r="C19" s="19"/>
+      <c r="D19" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="16"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="2:7" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>3.16</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="15" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16" t="s">
+      <c r="E20" s="14"/>
+      <c r="F20" s="15" t="s">
         <v>56</v>
       </c>
       <c r="G20" s="5"/>
@@ -992,108 +980,108 @@
       <c r="B21" s="4">
         <v>3.18</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="19"/>
+      <c r="D21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="12"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="2:7" s="2" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="18" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16" t="s">
+      <c r="E22" s="14"/>
+      <c r="F22" s="15" t="s">
         <v>52</v>
       </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="2:7" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="18" t="s">
+      <c r="C23" s="19"/>
+      <c r="D23" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16" t="s">
+      <c r="E23" s="14"/>
+      <c r="F23" s="15" t="s">
         <v>53</v>
       </c>
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="15" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="26" t="s">
+      <c r="E24" s="14"/>
+      <c r="F24" s="22" t="s">
         <v>51</v>
       </c>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="15" t="s">
+      <c r="C25" s="19"/>
+      <c r="D25" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="27"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="23"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="15" t="s">
+      <c r="C26" s="19"/>
+      <c r="D26" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="27"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="23"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="5" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="27"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="15" t="s">
+      <c r="C28" s="19"/>
+      <c r="D28" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="27"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="15" t="s">
+      <c r="C29" s="19"/>
+      <c r="D29" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="27"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="15" t="s">
+      <c r="C30" s="20"/>
+      <c r="D30" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="28"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="2:7" ht="120" x14ac:dyDescent="0.25">
@@ -1105,7 +1093,7 @@
         <v>45</v>
       </c>
       <c r="E31" s="9"/>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="12" t="s">
         <v>54</v>
       </c>
       <c r="G31" s="9"/>

</xml_diff>